<commit_message>
updates after new build
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2DCFF3-8865-451E-9950-59453C5A3493}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347EA340-E944-4DAF-A404-DB15AF5BAB83}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4980" yWindow="0" windowWidth="12945" windowHeight="14175" tabRatio="965" firstSheet="15" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14070" tabRatio="965" firstSheet="15" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6036" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6040" uniqueCount="275">
   <si>
     <t>customerID</t>
   </si>
@@ -878,6 +878,15 @@
   </si>
   <si>
     <t>Customer Test notes for AuTOMation</t>
+  </si>
+  <si>
+    <t>$40.00</t>
+  </si>
+  <si>
+    <t>amountDueSPA</t>
+  </si>
+  <si>
+    <t>amountDueBill</t>
   </si>
 </sst>
 </file>
@@ -8428,10 +8437,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60F061AC-4712-4967-896F-82F58A37D6C0}">
-  <dimension ref="A1:B134"/>
+  <dimension ref="A1:B136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8941,7 +8950,7 @@
         <v>39</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>51</v>
+        <v>272</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -8986,63 +8995,63 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>48</v>
+        <v>273</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>49</v>
+        <v>274</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>115</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>116</v>
+        <v>49</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>117</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>118</v>
+        <v>47</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>119</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>51</v>
+        <v>115</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>122</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>132</v>
+        <v>117</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>51</v>
@@ -9050,39 +9059,39 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>51</v>
+        <v>132</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>133</v>
+        <v>51</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>132</v>
+        <v>51</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>132</v>
@@ -9090,143 +9099,143 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>45</v>
+        <v>134</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>137</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>138</v>
+        <v>130</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>148</v>
+        <v>51</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>146</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>149</v>
+        <v>137</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>161</v>
+        <v>174</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>153</v>
+        <v>173</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>158</v>
@@ -9234,7 +9243,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>164</v>
@@ -9242,273 +9251,289 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>172</v>
+        <v>184</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
+        <v>190</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>191</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>192</v>
       </c>
-      <c r="B110" s="1" t="s">
+      <c r="B112" s="1" t="s">
         <v>188</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>233</v>
+        <v>190</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>234</v>
+        <v>186</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>187</v>
+        <v>234</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>188</v>
+        <v>235</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>239</v>
+        <v>187</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>240</v>
+        <v>188</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B134" s="1" t="s">
+      <c r="B136" s="1" t="s">
         <v>257</v>
       </c>
     </row>
@@ -14034,8 +14059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B737654-D179-4EEF-88A1-F71235BC78B5}">
   <dimension ref="A1:B110"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17265,13 +17290,13 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -17292,7 +17317,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B3" t="s">
         <v>271</v>
@@ -17300,7 +17325,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B4" t="s">
         <v>263</v>

</xml_diff>

<commit_message>
Updates , sikuli Image recognition
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347EA340-E944-4DAF-A404-DB15AF5BAB83}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3811E68A-8E67-4E4F-959C-4E0F8406AEAE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14070" tabRatio="965" firstSheet="15" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14070" tabRatio="965" firstSheet="15" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -25,32 +25,33 @@
     <sheet name="TC0014" sheetId="28" r:id="rId15"/>
     <sheet name="TC0015" sheetId="29" r:id="rId16"/>
     <sheet name="TC0016" sheetId="30" r:id="rId17"/>
-    <sheet name="TC0017" sheetId="31" r:id="rId18"/>
-    <sheet name="TC0018" sheetId="32" r:id="rId19"/>
-    <sheet name="TC0019" sheetId="33" r:id="rId20"/>
-    <sheet name="TC0020" sheetId="34" r:id="rId21"/>
-    <sheet name="TC0021" sheetId="35" r:id="rId22"/>
-    <sheet name="TC0022" sheetId="36" r:id="rId23"/>
-    <sheet name="TC0023" sheetId="37" r:id="rId24"/>
-    <sheet name="TC0024" sheetId="5" r:id="rId25"/>
-    <sheet name="TC0025" sheetId="6" r:id="rId26"/>
-    <sheet name="TC0026" sheetId="45" r:id="rId27"/>
-    <sheet name="TC0027" sheetId="46" r:id="rId28"/>
-    <sheet name="TC0028" sheetId="47" r:id="rId29"/>
-    <sheet name="TC0029" sheetId="52" r:id="rId30"/>
-    <sheet name="TC0030" sheetId="53" r:id="rId31"/>
-    <sheet name="TC0031" sheetId="54" r:id="rId32"/>
-    <sheet name="TC0032" sheetId="55" r:id="rId33"/>
-    <sheet name="TC0033" sheetId="56" r:id="rId34"/>
-    <sheet name="TC0034" sheetId="57" r:id="rId35"/>
-    <sheet name="TC0035" sheetId="58" r:id="rId36"/>
-    <sheet name="TC0036" sheetId="59" r:id="rId37"/>
-    <sheet name="TC0037" sheetId="48" r:id="rId38"/>
-    <sheet name="TC0038" sheetId="49" r:id="rId39"/>
-    <sheet name="TC0039" sheetId="50" r:id="rId40"/>
-    <sheet name="TC0040" sheetId="51" r:id="rId41"/>
-    <sheet name="TC0041" sheetId="60" r:id="rId42"/>
-    <sheet name="TC0042" sheetId="61" r:id="rId43"/>
+    <sheet name="TC0016_1" sheetId="62" r:id="rId18"/>
+    <sheet name="TC0017" sheetId="31" r:id="rId19"/>
+    <sheet name="TC0018" sheetId="32" r:id="rId20"/>
+    <sheet name="TC0019" sheetId="33" r:id="rId21"/>
+    <sheet name="TC0020" sheetId="34" r:id="rId22"/>
+    <sheet name="TC0021" sheetId="35" r:id="rId23"/>
+    <sheet name="TC0022" sheetId="36" r:id="rId24"/>
+    <sheet name="TC0023" sheetId="37" r:id="rId25"/>
+    <sheet name="TC0024" sheetId="5" r:id="rId26"/>
+    <sheet name="TC0025" sheetId="6" r:id="rId27"/>
+    <sheet name="TC0026" sheetId="45" r:id="rId28"/>
+    <sheet name="TC0027" sheetId="46" r:id="rId29"/>
+    <sheet name="TC0028" sheetId="47" r:id="rId30"/>
+    <sheet name="TC0029" sheetId="52" r:id="rId31"/>
+    <sheet name="TC0030" sheetId="53" r:id="rId32"/>
+    <sheet name="TC0031" sheetId="54" r:id="rId33"/>
+    <sheet name="TC0032" sheetId="55" r:id="rId34"/>
+    <sheet name="TC0033" sheetId="56" r:id="rId35"/>
+    <sheet name="TC0034" sheetId="57" r:id="rId36"/>
+    <sheet name="TC0035" sheetId="58" r:id="rId37"/>
+    <sheet name="TC0036" sheetId="59" r:id="rId38"/>
+    <sheet name="TC0037" sheetId="48" r:id="rId39"/>
+    <sheet name="TC0038" sheetId="49" r:id="rId40"/>
+    <sheet name="TC0039" sheetId="50" r:id="rId41"/>
+    <sheet name="TC0040" sheetId="51" r:id="rId42"/>
+    <sheet name="TC0041" sheetId="60" r:id="rId43"/>
+    <sheet name="TC0042" sheetId="61" r:id="rId44"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6040" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6050" uniqueCount="280">
   <si>
     <t>customerID</t>
   </si>
@@ -880,13 +881,28 @@
     <t>Customer Test notes for AuTOMation</t>
   </si>
   <si>
-    <t>$40.00</t>
+    <t>$120.00</t>
   </si>
   <si>
     <t>amountDueSPA</t>
   </si>
   <si>
     <t>amountDueBill</t>
+  </si>
+  <si>
+    <t>$75.26</t>
+  </si>
+  <si>
+    <t>Auto Customer</t>
+  </si>
+  <si>
+    <t>AUTO CUSTOM</t>
+  </si>
+  <si>
+    <t>BILLGRAPH</t>
+  </si>
+  <si>
+    <t>cus</t>
   </si>
 </sst>
 </file>
@@ -8439,8 +8455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60F061AC-4712-4967-896F-82F58A37D6C0}">
   <dimension ref="A1:B136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8998,7 +9014,7 @@
         <v>273</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>51</v>
+        <v>275</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -9006,7 +9022,7 @@
         <v>274</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>51</v>
+        <v>275</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -9546,6 +9562,65 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5956869-EB96-47C2-A44B-7B75D3BE73BF}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DDB3718-2C60-4822-87B8-352390D264A4}">
   <dimension ref="A1:B110"/>
   <sheetViews>
@@ -10442,908 +10517,6 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B34" r:id="rId1" xr:uid="{BB4A4236-43BF-4CBE-8CEA-5062F6EB00FD}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D747B1F-A6FD-4C84-822D-0FE661A51F45}">
-  <dimension ref="A1:B110"/>
-  <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="C120" sqref="C120"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" style="1" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B34" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>38</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>39</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>40</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>41</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>42</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>43</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>44</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>48</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>49</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>47</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>115</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>117</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>119</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>122</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>123</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>124</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>125</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>126</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>127</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>128</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>129</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>130</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>131</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>137</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>145</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>146</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>147</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>152</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>154</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>155</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>157</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>159</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>174</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>160</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>161</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>162</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>163</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>165</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>166</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>167</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>169</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>171</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>175</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>177</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>179</v>
-      </c>
-      <c r="B106" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>189</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>190</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>191</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>192</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B34" r:id="rId1" xr:uid="{A8404DB3-E56B-477E-A80A-86FDF4070140}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12252,6 +11425,908 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D747B1F-A6FD-4C84-822D-0FE661A51F45}">
+  <dimension ref="A1:B110"/>
+  <sheetViews>
+    <sheetView topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="C120" sqref="C120"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>38</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>39</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>40</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>41</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>42</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>43</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>44</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>48</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>49</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>47</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>115</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>117</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>119</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>122</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>123</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>124</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>125</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>126</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>127</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>128</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>129</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>130</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>131</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>137</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>145</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>146</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>147</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>152</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>154</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>155</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>157</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>159</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>174</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>160</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>161</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>162</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>163</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>165</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>166</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>167</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>169</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>171</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>175</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>177</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>179</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>189</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>190</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>191</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>192</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B34" r:id="rId1" xr:uid="{A8404DB3-E56B-477E-A80A-86FDF4070140}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E976AED-95E8-4C66-AB1C-989C534F26A3}">
   <dimension ref="A1:B110"/>
   <sheetViews>
@@ -13153,7 +13228,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9411933B-CF23-4B15-876D-FFB73E78CE94}">
   <dimension ref="A1:B110"/>
   <sheetViews>
@@ -14055,7 +14130,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B737654-D179-4EEF-88A1-F71235BC78B5}">
   <dimension ref="A1:B110"/>
   <sheetViews>
@@ -14957,7 +15032,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B418CC6E-ADAD-414D-90CD-F1B13BAFDD74}">
   <dimension ref="A1:B110"/>
   <sheetViews>
@@ -15859,7 +15934,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF9D265C-E875-4E14-9B57-5D6AEBC5DE7C}">
   <dimension ref="A1:B110"/>
   <sheetViews>
@@ -16761,7 +16836,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3177135D-A11B-4F80-B57E-F7BB77230313}">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -16844,7 +16919,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D295B29-90CD-483B-87F2-9D496E15A392}">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -16991,7 +17066,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3972B0C7-98E1-4EF2-A309-27683D8A9D22}">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -17138,7 +17213,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5611BD37-B66E-4BD2-A16B-2F4434459EDF}">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -17278,65 +17353,6 @@
       </c>
       <c r="B16" t="s">
         <v>227</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{127014DD-0DB6-46E8-A1F7-8A54D686BB94}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>262</v>
-      </c>
-      <c r="B3" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>261</v>
-      </c>
-      <c r="B4" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>192</v>
-      </c>
-      <c r="B5" t="s">
-        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -18248,6 +18264,65 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{127014DD-0DB6-46E8-A1F7-8A54D686BB94}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>262</v>
+      </c>
+      <c r="B3" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>261</v>
+      </c>
+      <c r="B4" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA759B7A-25E9-41B4-B822-73C3EC59C2C3}">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -18394,7 +18469,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E513CA-CBD0-49D5-9332-0CDCD76301DB}">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -18541,7 +18616,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6B37A4C-A05C-4809-AE2C-D6D1680F7500}">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -18688,7 +18763,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D56D8C-BEE9-4C9A-A805-1A2AB98435C2}">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -18835,7 +18910,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60DCDD80-5E3D-4A40-86EE-DB691496C38D}">
   <dimension ref="A1:B18"/>
   <sheetViews>
@@ -18998,7 +19073,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCADEDFC-6649-4AA8-9375-9AB761BBA1DC}">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -19148,7 +19223,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2532673-A32D-4783-8152-7D76B1BE5FEB}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -19215,7 +19290,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{324AA46E-4E2F-4D5C-9BA4-2A0ADBB857EA}">
   <dimension ref="A1:B18"/>
   <sheetViews>
@@ -19378,7 +19453,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B4CA557-2CD6-4153-86EB-47E0FFCC258C}">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -19517,73 +19592,6 @@
         <v>228</v>
       </c>
       <c r="B16" t="s">
-        <v>227</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F300FDA-518E-44AE-8FA4-DADE3D8F9158}">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>203</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>268</v>
-      </c>
-      <c r="B4" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>269</v>
-      </c>
-      <c r="B5" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>228</v>
-      </c>
-      <c r="B6" t="s">
         <v>227</v>
       </c>
     </row>
@@ -20495,6 +20503,73 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F300FDA-518E-44AE-8FA4-DADE3D8F9158}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>268</v>
+      </c>
+      <c r="B4" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>269</v>
+      </c>
+      <c r="B5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>228</v>
+      </c>
+      <c r="B6" t="s">
+        <v>227</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B4A285C-74F4-43B9-939E-A6C03484F25F}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -20553,7 +20628,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E45FD00-34C1-4731-9C4C-186CB9F63E7B}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -20612,7 +20687,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84E27F34-BE30-49BD-B842-082702198BEA}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -20671,7 +20746,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCE24B47-E282-4484-BB3C-4E5B3D705BAB}">
   <dimension ref="A1:B134"/>
   <sheetViews>

</xml_diff>

<commit_message>
added accounts case for refresh page
added accounts case for refresh page
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A601D7F-82F8-4F78-A903-82F149877DE7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630ACFBA-6426-47F5-9F2A-BAA7AEB4E574}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14070" tabRatio="965" firstSheet="15" activeTab="31" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14415" tabRatio="965" firstSheet="9" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -17,41 +17,42 @@
     <sheet name="TC0006" sheetId="20" r:id="rId7"/>
     <sheet name="TC0007" sheetId="21" r:id="rId8"/>
     <sheet name="TC0008" sheetId="22" r:id="rId9"/>
-    <sheet name="TC0009" sheetId="23" r:id="rId10"/>
-    <sheet name="TC0010" sheetId="24" r:id="rId11"/>
-    <sheet name="TC0011" sheetId="25" r:id="rId12"/>
-    <sheet name="TC0012" sheetId="26" r:id="rId13"/>
-    <sheet name="TC0013" sheetId="27" r:id="rId14"/>
-    <sheet name="TC0014" sheetId="28" r:id="rId15"/>
-    <sheet name="TC0015" sheetId="29" r:id="rId16"/>
-    <sheet name="TC0016" sheetId="30" r:id="rId17"/>
-    <sheet name="TC0016_1" sheetId="62" r:id="rId18"/>
-    <sheet name="TC0017" sheetId="31" r:id="rId19"/>
-    <sheet name="TC0018" sheetId="32" r:id="rId20"/>
-    <sheet name="TC0019" sheetId="33" r:id="rId21"/>
-    <sheet name="TC0020" sheetId="34" r:id="rId22"/>
-    <sheet name="TC0021" sheetId="35" r:id="rId23"/>
-    <sheet name="TC0022" sheetId="36" r:id="rId24"/>
-    <sheet name="TC0023" sheetId="37" r:id="rId25"/>
-    <sheet name="TC0024" sheetId="5" r:id="rId26"/>
-    <sheet name="TC0025" sheetId="6" r:id="rId27"/>
-    <sheet name="TC0026" sheetId="45" r:id="rId28"/>
-    <sheet name="TC0027" sheetId="46" r:id="rId29"/>
-    <sheet name="TC0028" sheetId="47" r:id="rId30"/>
-    <sheet name="TC0029" sheetId="52" r:id="rId31"/>
-    <sheet name="TC0030" sheetId="53" r:id="rId32"/>
-    <sheet name="TC0031" sheetId="54" r:id="rId33"/>
-    <sheet name="TC0032" sheetId="55" r:id="rId34"/>
-    <sheet name="TC0033" sheetId="56" r:id="rId35"/>
-    <sheet name="TC0034" sheetId="57" r:id="rId36"/>
-    <sheet name="TC0035" sheetId="58" r:id="rId37"/>
-    <sheet name="TC0036" sheetId="59" r:id="rId38"/>
-    <sheet name="TC0037" sheetId="48" r:id="rId39"/>
-    <sheet name="TC0038" sheetId="49" r:id="rId40"/>
-    <sheet name="TC0039" sheetId="50" r:id="rId41"/>
-    <sheet name="TC0040" sheetId="51" r:id="rId42"/>
-    <sheet name="TC0041" sheetId="60" r:id="rId43"/>
-    <sheet name="TC0042" sheetId="61" r:id="rId44"/>
+    <sheet name="TC0009_1" sheetId="63" r:id="rId10"/>
+    <sheet name="TC0009" sheetId="23" r:id="rId11"/>
+    <sheet name="TC0010" sheetId="24" r:id="rId12"/>
+    <sheet name="TC0011" sheetId="25" r:id="rId13"/>
+    <sheet name="TC0012" sheetId="26" r:id="rId14"/>
+    <sheet name="TC0013" sheetId="27" r:id="rId15"/>
+    <sheet name="TC0014" sheetId="28" r:id="rId16"/>
+    <sheet name="TC0015" sheetId="29" r:id="rId17"/>
+    <sheet name="TC0016" sheetId="30" r:id="rId18"/>
+    <sheet name="TC0016_1" sheetId="62" r:id="rId19"/>
+    <sheet name="TC0017" sheetId="31" r:id="rId20"/>
+    <sheet name="TC0018" sheetId="32" r:id="rId21"/>
+    <sheet name="TC0019" sheetId="33" r:id="rId22"/>
+    <sheet name="TC0020" sheetId="34" r:id="rId23"/>
+    <sheet name="TC0021" sheetId="35" r:id="rId24"/>
+    <sheet name="TC0022" sheetId="36" r:id="rId25"/>
+    <sheet name="TC0023" sheetId="37" r:id="rId26"/>
+    <sheet name="TC0024" sheetId="5" r:id="rId27"/>
+    <sheet name="TC0025" sheetId="6" r:id="rId28"/>
+    <sheet name="TC0026" sheetId="45" r:id="rId29"/>
+    <sheet name="TC0027" sheetId="46" r:id="rId30"/>
+    <sheet name="TC0028" sheetId="47" r:id="rId31"/>
+    <sheet name="TC0029" sheetId="52" r:id="rId32"/>
+    <sheet name="TC0030" sheetId="53" r:id="rId33"/>
+    <sheet name="TC0031" sheetId="54" r:id="rId34"/>
+    <sheet name="TC0032" sheetId="55" r:id="rId35"/>
+    <sheet name="TC0033" sheetId="56" r:id="rId36"/>
+    <sheet name="TC0034" sheetId="57" r:id="rId37"/>
+    <sheet name="TC0035" sheetId="58" r:id="rId38"/>
+    <sheet name="TC0036" sheetId="59" r:id="rId39"/>
+    <sheet name="TC0037" sheetId="48" r:id="rId40"/>
+    <sheet name="TC0038" sheetId="49" r:id="rId41"/>
+    <sheet name="TC0039" sheetId="50" r:id="rId42"/>
+    <sheet name="TC0040" sheetId="51" r:id="rId43"/>
+    <sheet name="TC0041" sheetId="60" r:id="rId44"/>
+    <sheet name="TC0042" sheetId="61" r:id="rId45"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -63,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6052" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6282" uniqueCount="291">
   <si>
     <t>customerID</t>
   </si>
@@ -909,6 +910,33 @@
   </si>
   <si>
     <t>$80.00</t>
+  </si>
+  <si>
+    <t>accAddLine2</t>
+  </si>
+  <si>
+    <t>accAddCity2</t>
+  </si>
+  <si>
+    <t>accAddState2</t>
+  </si>
+  <si>
+    <t>accAddZip2</t>
+  </si>
+  <si>
+    <t>accAddId2</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Ny</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>89218-3</t>
   </si>
 </sst>
 </file>
@@ -2144,10 +2172,952 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75403725-5D2C-4D57-B728-F6EE33CC1353}">
+  <dimension ref="A1:B115"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>38</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>39</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>40</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>41</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>42</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>43</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>44</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>48</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>49</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>47</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>115</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>117</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>119</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>122</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>123</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>124</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>125</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>126</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>127</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>128</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>129</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>130</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>131</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>137</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>145</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>146</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>147</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>152</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>154</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>155</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>157</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>159</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>174</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>160</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>161</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>162</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>163</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>165</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>166</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>167</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>169</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>171</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>175</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>177</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>179</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>189</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>190</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>191</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>192</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B34" r:id="rId1" xr:uid="{7C5E1420-F61F-4CF9-B1EA-064838A4743A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FF65505-0DC8-4A83-B5EF-9CDAAEF55EAC}">
   <dimension ref="A1:B110"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
+    <sheetView topLeftCell="A88" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -3045,7 +4015,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BDE68CA-DFC7-438F-B310-89CF22A4930D}">
   <dimension ref="A1:B110"/>
   <sheetViews>
@@ -3947,7 +4917,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F41C021-45AC-4C59-9EC5-6BE743228B60}">
   <dimension ref="A1:B110"/>
   <sheetViews>
@@ -4849,7 +5819,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4897A1AA-71CC-4A94-BF68-D6EE809AB8AE}">
   <dimension ref="A1:B110"/>
   <sheetViews>
@@ -5751,7 +6721,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E31CEF9-5F72-47AA-A14C-28060C69FA37}">
   <dimension ref="A1:B110"/>
   <sheetViews>
@@ -6653,7 +7623,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B7A780-A8BA-4F3F-97E4-CB405115845A}">
   <dimension ref="A1:B110"/>
   <sheetViews>
@@ -7555,7 +8525,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A50CEE85-26CF-4FC6-9301-CFBA4ABD5CAB}">
   <dimension ref="A1:B110"/>
   <sheetViews>
@@ -8457,7 +9427,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60F061AC-4712-4967-896F-82F58A37D6C0}">
   <dimension ref="A1:B137"/>
   <sheetViews>
@@ -9575,7 +10545,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5956869-EB96-47C2-A44B-7B75D3BE73BF}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -9630,908 +10600,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DDB3718-2C60-4822-87B8-352390D264A4}">
-  <dimension ref="A1:B110"/>
-  <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" style="1" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B34" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>38</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>39</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>40</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>41</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>42</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>43</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>44</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>48</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>49</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>47</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>115</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>117</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>119</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>122</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>123</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>124</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>125</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>126</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>127</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>128</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>129</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>130</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>131</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>137</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>145</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>146</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>147</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>152</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>154</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>155</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>157</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>159</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>174</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>160</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>161</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>162</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>163</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>165</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>166</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>167</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>169</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>171</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>175</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>177</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>179</v>
-      </c>
-      <c r="B106" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>189</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>190</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>191</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>192</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B34" r:id="rId1" xr:uid="{BB4A4236-43BF-4CBE-8CEA-5062F6EB00FD}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -11439,6 +11507,908 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DDB3718-2C60-4822-87B8-352390D264A4}">
+  <dimension ref="A1:B110"/>
+  <sheetViews>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>38</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>39</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>40</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>41</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>42</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>43</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>44</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>48</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>49</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>47</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>115</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>117</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>119</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>122</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>123</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>124</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>125</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>126</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>127</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>128</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>129</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>130</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>131</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>137</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>145</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>146</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>147</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>152</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>154</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>155</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>157</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>159</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>174</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>160</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>161</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>162</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>163</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>165</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>166</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>167</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>169</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>171</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>175</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>177</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>179</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>189</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>190</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>191</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>192</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B34" r:id="rId1" xr:uid="{BB4A4236-43BF-4CBE-8CEA-5062F6EB00FD}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D747B1F-A6FD-4C84-822D-0FE661A51F45}">
   <dimension ref="A1:B110"/>
   <sheetViews>
@@ -12340,7 +13310,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E976AED-95E8-4C66-AB1C-989C534F26A3}">
   <dimension ref="A1:B110"/>
   <sheetViews>
@@ -13242,7 +14212,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9411933B-CF23-4B15-876D-FFB73E78CE94}">
   <dimension ref="A1:B110"/>
   <sheetViews>
@@ -14144,7 +15114,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B737654-D179-4EEF-88A1-F71235BC78B5}">
   <dimension ref="A1:B110"/>
   <sheetViews>
@@ -15046,7 +16016,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B418CC6E-ADAD-414D-90CD-F1B13BAFDD74}">
   <dimension ref="A1:B110"/>
   <sheetViews>
@@ -15948,7 +16918,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF9D265C-E875-4E14-9B57-5D6AEBC5DE7C}">
   <dimension ref="A1:B110"/>
   <sheetViews>
@@ -16850,7 +17820,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3177135D-A11B-4F80-B57E-F7BB77230313}">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -16933,7 +17903,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D295B29-90CD-483B-87F2-9D496E15A392}">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -17080,159 +18050,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3972B0C7-98E1-4EF2-A309-27683D8A9D22}">
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>203</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>205</v>
-      </c>
-      <c r="B4" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>206</v>
-      </c>
-      <c r="B5" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>209</v>
-      </c>
-      <c r="B6" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>210</v>
-      </c>
-      <c r="B7" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>212</v>
-      </c>
-      <c r="B8" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>214</v>
-      </c>
-      <c r="B9" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>216</v>
-      </c>
-      <c r="B10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>217</v>
-      </c>
-      <c r="B11" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>219</v>
-      </c>
-      <c r="B12" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>221</v>
-      </c>
-      <c r="B13" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>223</v>
-      </c>
-      <c r="B14" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>225</v>
-      </c>
-      <c r="B15" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>228</v>
-      </c>
-      <c r="B16" t="s">
-        <v>227</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5611BD37-B66E-4BD2-A16B-2F4434459EDF}">
-  <dimension ref="A1:B16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18278,6 +19101,153 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5611BD37-B66E-4BD2-A16B-2F4434459EDF}">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>206</v>
+      </c>
+      <c r="B5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>209</v>
+      </c>
+      <c r="B6" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>210</v>
+      </c>
+      <c r="B7" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>212</v>
+      </c>
+      <c r="B8" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>214</v>
+      </c>
+      <c r="B9" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>216</v>
+      </c>
+      <c r="B10" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>217</v>
+      </c>
+      <c r="B11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>219</v>
+      </c>
+      <c r="B12" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>221</v>
+      </c>
+      <c r="B13" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>223</v>
+      </c>
+      <c r="B14" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>225</v>
+      </c>
+      <c r="B15" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>228</v>
+      </c>
+      <c r="B16" t="s">
+        <v>227</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{127014DD-0DB6-46E8-A1F7-8A54D686BB94}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -18336,7 +19306,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA759B7A-25E9-41B4-B822-73C3EC59C2C3}">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -18483,12 +19453,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E513CA-CBD0-49D5-9332-0CDCD76301DB}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18630,7 +19600,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6B37A4C-A05C-4809-AE2C-D6D1680F7500}">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -18777,7 +19747,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D56D8C-BEE9-4C9A-A805-1A2AB98435C2}">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -18924,7 +19894,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60DCDD80-5E3D-4A40-86EE-DB691496C38D}">
   <dimension ref="A1:B18"/>
   <sheetViews>
@@ -19087,7 +20057,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCADEDFC-6649-4AA8-9375-9AB761BBA1DC}">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -19237,7 +20207,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2532673-A32D-4783-8152-7D76B1BE5FEB}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -19304,7 +20274,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{324AA46E-4E2F-4D5C-9BA4-2A0ADBB857EA}">
   <dimension ref="A1:B18"/>
   <sheetViews>
@@ -19460,153 +20430,6 @@
       </c>
       <c r="B18" t="s">
         <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B4CA557-2CD6-4153-86EB-47E0FFCC258C}">
-  <dimension ref="A1:B16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>203</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>205</v>
-      </c>
-      <c r="B4" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>206</v>
-      </c>
-      <c r="B5" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>209</v>
-      </c>
-      <c r="B6" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>210</v>
-      </c>
-      <c r="B7" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>212</v>
-      </c>
-      <c r="B8" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>214</v>
-      </c>
-      <c r="B9" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>216</v>
-      </c>
-      <c r="B10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>217</v>
-      </c>
-      <c r="B11" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>219</v>
-      </c>
-      <c r="B12" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>221</v>
-      </c>
-      <c r="B13" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>223</v>
-      </c>
-      <c r="B14" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>225</v>
-      </c>
-      <c r="B15" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>228</v>
-      </c>
-      <c r="B16" t="s">
-        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -20517,6 +21340,153 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B4CA557-2CD6-4153-86EB-47E0FFCC258C}">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>206</v>
+      </c>
+      <c r="B5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>209</v>
+      </c>
+      <c r="B6" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>210</v>
+      </c>
+      <c r="B7" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>212</v>
+      </c>
+      <c r="B8" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>214</v>
+      </c>
+      <c r="B9" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>216</v>
+      </c>
+      <c r="B10" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>217</v>
+      </c>
+      <c r="B11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>219</v>
+      </c>
+      <c r="B12" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>221</v>
+      </c>
+      <c r="B13" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>223</v>
+      </c>
+      <c r="B14" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>225</v>
+      </c>
+      <c r="B15" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>228</v>
+      </c>
+      <c r="B16" t="s">
+        <v>227</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F300FDA-518E-44AE-8FA4-DADE3D8F9158}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -20583,7 +21553,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B4A285C-74F4-43B9-939E-A6C03484F25F}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -20642,7 +21612,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E45FD00-34C1-4731-9C4C-186CB9F63E7B}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -20701,7 +21671,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84E27F34-BE30-49BD-B842-082702198BEA}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -20760,7 +21730,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCE24B47-E282-4484-BB3C-4E5B3D705BAB}">
   <dimension ref="A1:B134"/>
   <sheetViews>

</xml_diff>

<commit_message>
order by bill datae scripts added
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630ACFBA-6426-47F5-9F2A-BAA7AEB4E574}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31071E67-D115-494E-8AE8-ECCB79FE94F4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14415" tabRatio="965" firstSheet="9" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14415" tabRatio="965" firstSheet="9" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -28,33 +28,34 @@
     <sheet name="TC0016" sheetId="30" r:id="rId18"/>
     <sheet name="TC0016_1" sheetId="62" r:id="rId19"/>
     <sheet name="TC0017" sheetId="31" r:id="rId20"/>
-    <sheet name="TC0018" sheetId="32" r:id="rId21"/>
-    <sheet name="TC0019" sheetId="33" r:id="rId22"/>
-    <sheet name="TC0020" sheetId="34" r:id="rId23"/>
-    <sheet name="TC0021" sheetId="35" r:id="rId24"/>
-    <sheet name="TC0022" sheetId="36" r:id="rId25"/>
-    <sheet name="TC0023" sheetId="37" r:id="rId26"/>
-    <sheet name="TC0024" sheetId="5" r:id="rId27"/>
-    <sheet name="TC0025" sheetId="6" r:id="rId28"/>
-    <sheet name="TC0026" sheetId="45" r:id="rId29"/>
-    <sheet name="TC0027" sheetId="46" r:id="rId30"/>
-    <sheet name="TC0028" sheetId="47" r:id="rId31"/>
-    <sheet name="TC0029" sheetId="52" r:id="rId32"/>
-    <sheet name="TC0030" sheetId="53" r:id="rId33"/>
-    <sheet name="TC0031" sheetId="54" r:id="rId34"/>
-    <sheet name="TC0032" sheetId="55" r:id="rId35"/>
-    <sheet name="TC0033" sheetId="56" r:id="rId36"/>
-    <sheet name="TC0034" sheetId="57" r:id="rId37"/>
-    <sheet name="TC0035" sheetId="58" r:id="rId38"/>
-    <sheet name="TC0036" sheetId="59" r:id="rId39"/>
-    <sheet name="TC0037" sheetId="48" r:id="rId40"/>
-    <sheet name="TC0038" sheetId="49" r:id="rId41"/>
-    <sheet name="TC0039" sheetId="50" r:id="rId42"/>
-    <sheet name="TC0040" sheetId="51" r:id="rId43"/>
-    <sheet name="TC0041" sheetId="60" r:id="rId44"/>
-    <sheet name="TC0042" sheetId="61" r:id="rId45"/>
+    <sheet name="TC0017_1" sheetId="64" r:id="rId21"/>
+    <sheet name="TC0018" sheetId="32" r:id="rId22"/>
+    <sheet name="TC0019" sheetId="33" r:id="rId23"/>
+    <sheet name="TC0020" sheetId="34" r:id="rId24"/>
+    <sheet name="TC0021" sheetId="35" r:id="rId25"/>
+    <sheet name="TC0022" sheetId="36" r:id="rId26"/>
+    <sheet name="TC0023" sheetId="37" r:id="rId27"/>
+    <sheet name="TC0024" sheetId="5" r:id="rId28"/>
+    <sheet name="TC0025" sheetId="6" r:id="rId29"/>
+    <sheet name="TC0026" sheetId="45" r:id="rId30"/>
+    <sheet name="TC0027" sheetId="46" r:id="rId31"/>
+    <sheet name="TC0028" sheetId="47" r:id="rId32"/>
+    <sheet name="TC0029" sheetId="52" r:id="rId33"/>
+    <sheet name="TC0030" sheetId="53" r:id="rId34"/>
+    <sheet name="TC0031" sheetId="54" r:id="rId35"/>
+    <sheet name="TC0032" sheetId="55" r:id="rId36"/>
+    <sheet name="TC0033" sheetId="56" r:id="rId37"/>
+    <sheet name="TC0034" sheetId="57" r:id="rId38"/>
+    <sheet name="TC0035" sheetId="58" r:id="rId39"/>
+    <sheet name="TC0036" sheetId="59" r:id="rId40"/>
+    <sheet name="TC0037" sheetId="48" r:id="rId41"/>
+    <sheet name="TC0038" sheetId="49" r:id="rId42"/>
+    <sheet name="TC0039" sheetId="50" r:id="rId43"/>
+    <sheet name="TC0040" sheetId="51" r:id="rId44"/>
+    <sheet name="TC0041" sheetId="60" r:id="rId45"/>
+    <sheet name="TC0042" sheetId="61" r:id="rId46"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6282" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6508" uniqueCount="299">
   <si>
     <t>customerID</t>
   </si>
@@ -937,6 +938,30 @@
   </si>
   <si>
     <t>89218-3</t>
+  </si>
+  <si>
+    <t>SEWER001</t>
+  </si>
+  <si>
+    <t>stDateValue2</t>
+  </si>
+  <si>
+    <t>stDateValue3</t>
+  </si>
+  <si>
+    <t>stDateValue4</t>
+  </si>
+  <si>
+    <t>Aug 31, 1998</t>
+  </si>
+  <si>
+    <t>Jun 30, 1998</t>
+  </si>
+  <si>
+    <t>Apr 30, 1998</t>
+  </si>
+  <si>
+    <t>Feb 28, 1998</t>
   </si>
 </sst>
 </file>
@@ -2175,7 +2200,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75403725-5D2C-4D57-B728-F6EE33CC1353}">
   <dimension ref="A1:B115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
@@ -11510,8 +11535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DDB3718-2C60-4822-87B8-352390D264A4}">
   <dimension ref="A1:B110"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A30" sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12409,6 +12434,932 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC6E2D24-026B-4558-84B8-111FA2AEC5C6}">
+  <dimension ref="A1:B113"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>38</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>39</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>40</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>41</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>42</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>43</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>44</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>48</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>49</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>47</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>115</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>117</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>119</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>122</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>123</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>124</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>125</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>126</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>127</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>128</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>129</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>130</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>131</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>137</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>145</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>146</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>147</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>152</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>154</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>155</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>157</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>159</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>174</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>160</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>161</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>162</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>163</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>165</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>166</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>167</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>169</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>171</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>175</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>177</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>179</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>189</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>190</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>191</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>192</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B34" r:id="rId1" xr:uid="{DF90CC5B-1471-4AB1-A22D-B2EECE6941D0}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D747B1F-A6FD-4C84-822D-0FE661A51F45}">
   <dimension ref="A1:B110"/>
   <sheetViews>
@@ -13310,7 +14261,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E976AED-95E8-4C66-AB1C-989C534F26A3}">
   <dimension ref="A1:B110"/>
   <sheetViews>
@@ -14212,7 +15163,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9411933B-CF23-4B15-876D-FFB73E78CE94}">
   <dimension ref="A1:B110"/>
   <sheetViews>
@@ -15114,7 +16065,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B737654-D179-4EEF-88A1-F71235BC78B5}">
   <dimension ref="A1:B110"/>
   <sheetViews>
@@ -16016,7 +16967,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B418CC6E-ADAD-414D-90CD-F1B13BAFDD74}">
   <dimension ref="A1:B110"/>
   <sheetViews>
@@ -16918,7 +17869,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF9D265C-E875-4E14-9B57-5D6AEBC5DE7C}">
   <dimension ref="A1:B110"/>
   <sheetViews>
@@ -17820,7 +18771,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3177135D-A11B-4F80-B57E-F7BB77230313}">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -17903,7 +18854,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D295B29-90CD-483B-87F2-9D496E15A392}">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -17915,153 +18866,6 @@
   <cols>
     <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>203</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>205</v>
-      </c>
-      <c r="B4" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>206</v>
-      </c>
-      <c r="B5" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>209</v>
-      </c>
-      <c r="B6" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>210</v>
-      </c>
-      <c r="B7" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>212</v>
-      </c>
-      <c r="B8" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>214</v>
-      </c>
-      <c r="B9" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>216</v>
-      </c>
-      <c r="B10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>217</v>
-      </c>
-      <c r="B11" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>219</v>
-      </c>
-      <c r="B12" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>221</v>
-      </c>
-      <c r="B13" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>223</v>
-      </c>
-      <c r="B14" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>225</v>
-      </c>
-      <c r="B15" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>228</v>
-      </c>
-      <c r="B16" t="s">
-        <v>227</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3972B0C7-98E1-4EF2-A309-27683D8A9D22}">
-  <dimension ref="A1:B16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -19101,6 +19905,153 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3972B0C7-98E1-4EF2-A309-27683D8A9D22}">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>206</v>
+      </c>
+      <c r="B5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>209</v>
+      </c>
+      <c r="B6" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>210</v>
+      </c>
+      <c r="B7" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>212</v>
+      </c>
+      <c r="B8" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>214</v>
+      </c>
+      <c r="B9" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>216</v>
+      </c>
+      <c r="B10" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>217</v>
+      </c>
+      <c r="B11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>219</v>
+      </c>
+      <c r="B12" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>221</v>
+      </c>
+      <c r="B13" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>223</v>
+      </c>
+      <c r="B14" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>225</v>
+      </c>
+      <c r="B15" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>228</v>
+      </c>
+      <c r="B16" t="s">
+        <v>227</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5611BD37-B66E-4BD2-A16B-2F4434459EDF}">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -19247,7 +20198,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{127014DD-0DB6-46E8-A1F7-8A54D686BB94}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -19306,7 +20257,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA759B7A-25E9-41B4-B822-73C3EC59C2C3}">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -19453,7 +20404,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E513CA-CBD0-49D5-9332-0CDCD76301DB}">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -19600,7 +20551,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6B37A4C-A05C-4809-AE2C-D6D1680F7500}">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -19747,7 +20698,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D56D8C-BEE9-4C9A-A805-1A2AB98435C2}">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -19894,7 +20845,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60DCDD80-5E3D-4A40-86EE-DB691496C38D}">
   <dimension ref="A1:B18"/>
   <sheetViews>
@@ -20057,7 +21008,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCADEDFC-6649-4AA8-9375-9AB761BBA1DC}">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -20207,7 +21158,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2532673-A32D-4783-8152-7D76B1BE5FEB}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -20267,169 +21218,6 @@
       </c>
       <c r="B6" t="s">
         <v>266</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{324AA46E-4E2F-4D5C-9BA4-2A0ADBB857EA}">
-  <dimension ref="A1:B18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>203</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>205</v>
-      </c>
-      <c r="B4" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>206</v>
-      </c>
-      <c r="B5" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>209</v>
-      </c>
-      <c r="B6" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>210</v>
-      </c>
-      <c r="B7" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>212</v>
-      </c>
-      <c r="B8" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>214</v>
-      </c>
-      <c r="B9" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>216</v>
-      </c>
-      <c r="B10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>217</v>
-      </c>
-      <c r="B11" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>219</v>
-      </c>
-      <c r="B12" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>221</v>
-      </c>
-      <c r="B13" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>223</v>
-      </c>
-      <c r="B14" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>225</v>
-      </c>
-      <c r="B15" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>228</v>
-      </c>
-      <c r="B16" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>264</v>
-      </c>
-      <c r="B17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>265</v>
-      </c>
-      <c r="B18" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -21340,6 +22128,169 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{324AA46E-4E2F-4D5C-9BA4-2A0ADBB857EA}">
+  <dimension ref="A1:B18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>206</v>
+      </c>
+      <c r="B5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>209</v>
+      </c>
+      <c r="B6" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>210</v>
+      </c>
+      <c r="B7" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>212</v>
+      </c>
+      <c r="B8" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>214</v>
+      </c>
+      <c r="B9" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>216</v>
+      </c>
+      <c r="B10" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>217</v>
+      </c>
+      <c r="B11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>219</v>
+      </c>
+      <c r="B12" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>221</v>
+      </c>
+      <c r="B13" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>223</v>
+      </c>
+      <c r="B14" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>225</v>
+      </c>
+      <c r="B15" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>228</v>
+      </c>
+      <c r="B16" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>264</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>265</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B4CA557-2CD6-4153-86EB-47E0FFCC258C}">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -21486,7 +22437,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F300FDA-518E-44AE-8FA4-DADE3D8F9158}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -21553,7 +22504,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B4A285C-74F4-43B9-939E-A6C03484F25F}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -21612,7 +22563,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E45FD00-34C1-4731-9C4C-186CB9F63E7B}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -21671,7 +22622,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84E27F34-BE30-49BD-B842-082702198BEA}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -21730,7 +22681,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCE24B47-E282-4484-BB3C-4E5B3D705BAB}">
   <dimension ref="A1:B134"/>
   <sheetViews>

</xml_diff>